<commit_message>
informe final 3 - terminado
</commit_message>
<xml_diff>
--- a/3. IDENTIFICACION PARAMETROS/INFORME PREVIO/calculo_parametros.xlsx
+++ b/3. IDENTIFICACION PARAMETROS/INFORME PREVIO/calculo_parametros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bremdows\UNSAAC\SEMESTRE VIII\lab-control-i\3. IDENTIFICACION PARAMETROS\INFORME PREVIO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNSAAC\SEMESTRE VIII\lab-control-i\3. IDENTIFICACION PARAMETROS\INFORME PREVIO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42B15C12-42AB-46CF-AA53-BF1666158779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD94842-9417-48D4-85EB-43AB709BDD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="11520" windowHeight="12504" xr2:uid="{ADB2C703-5703-4219-8002-D3874C9FF231}"/>
+    <workbookView xWindow="5820" yWindow="1080" windowWidth="21225" windowHeight="13665" xr2:uid="{ADB2C703-5703-4219-8002-D3874C9FF231}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>J</t>
   </si>
@@ -63,14 +61,63 @@
   </si>
   <si>
     <t>S^1</t>
+  </si>
+  <si>
+    <t>Num</t>
+  </si>
+  <si>
+    <t>Deno</t>
+  </si>
+  <si>
+    <t>S^0</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Wn</t>
+  </si>
+  <si>
+    <t>Xi</t>
+  </si>
+  <si>
+    <t>Ts</t>
+  </si>
+  <si>
+    <t>Te</t>
+  </si>
+  <si>
+    <t>Regla de tres</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -98,8 +145,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,18 +466,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE12529-7763-4EF0-93E4-73E6F0B85284}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,7 +487,7 @@
         <v>1.5999999999999999E-6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -443,7 +496,7 @@
         <v>9.3500000000000007E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -451,7 +504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -459,7 +512,7 @@
         <v>4.36E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -467,7 +520,7 @@
         <v>4.36E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -476,18 +529,18 @@
         <v>1.3999999999999999E-6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f>B1*B2</f>
         <v>1.496E-8</v>
@@ -499,6 +552,128 @@
       <c r="C10">
         <f>(B6*B3)+(B4*B5)</f>
         <v>1.92476E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <f>B5/A10</f>
+        <v>2914438.5026737968</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <f>C13/D15</f>
+        <v>22.65217481660051</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <f>SQRT(D15)</f>
+        <v>358.69266483646783</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <f>B10/A10</f>
+        <v>1819.056818181818</v>
+      </c>
+      <c r="D15">
+        <f>C10/A10</f>
+        <v>128660.42780748663</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <f>C15/(2*G14)</f>
+        <v>2.5356760766367321</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16">
+        <f>2*G15/G14</f>
+        <v>1.4138432843575301E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <f>G16*4</f>
+        <v>5.6553731374301204E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>22.06</v>
+      </c>
+      <c r="B20">
+        <f>A20*100/22.65</f>
+        <v>97.395143487858732</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>14.226000000000001</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ref="B21:B23" si="0">A21*100/22.65</f>
+        <v>62.807947019867562</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>14.82</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>65.430463576158942</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>